<commit_message>
Update $DKNG with more data, calculate some metrics
</commit_message>
<xml_diff>
--- a/$DKNG.xlsx
+++ b/$DKNG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0213351B-DEC7-4677-81A5-5FA6BA52013E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5421C-D4E4-7B4A-9245-4A277741C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16695" xr2:uid="{E77186FA-83D4-479E-A0A9-B880EBEEF096}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18900" xr2:uid="{E77186FA-83D4-479E-A0A9-B880EBEEF096}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="114">
   <si>
     <t>$DKNG</t>
   </si>
@@ -163,9 +173,6 @@
     <t>Revenue % Y/Y</t>
   </si>
   <si>
-    <t>Revenue % H/H</t>
-  </si>
-  <si>
     <t>Balance Sheet</t>
   </si>
   <si>
@@ -344,15 +351,43 @@
   </si>
   <si>
     <t>Other Liabilities</t>
+  </si>
+  <si>
+    <t>Revenue % Q/Q</t>
+  </si>
+  <si>
+    <t>Book Value</t>
+  </si>
+  <si>
+    <t>Book Value per Share</t>
+  </si>
+  <si>
+    <t>Share Price</t>
+  </si>
+  <si>
+    <t>P/B</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>EV/S</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>Key Metrics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -577,7 +612,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -614,7 +649,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -637,7 +671,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -652,15 +686,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -678,8 +703,29 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -688,17 +734,24 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -717,16 +770,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>368301</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>100023</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -756,8 +809,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3657600" y="161925"/>
-          <a:ext cx="2095500" cy="1057275"/>
+          <a:off x="1765301" y="63500"/>
+          <a:ext cx="1128722" cy="508000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -778,14 +831,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>77395</xdr:rowOff>
     </xdr:to>
@@ -817,8 +870,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8677275" y="161925"/>
-          <a:ext cx="5524500" cy="4639870"/>
+          <a:off x="11023600" y="165100"/>
+          <a:ext cx="6324600" cy="4725595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -852,8 +905,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -868,8 +921,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9159875" y="0"/>
-          <a:ext cx="0" cy="9061450"/>
+          <a:off x="10382250" y="0"/>
+          <a:ext cx="0" cy="14922500"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -902,8 +955,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -918,8 +971,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9813925" y="0"/>
-          <a:ext cx="0" cy="9398000"/>
+          <a:off x="14728825" y="0"/>
+          <a:ext cx="0" cy="14757400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1242,49 +1295,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72920D05-7E62-4C8A-A716-46BB4747797C}">
-  <dimension ref="B2:O27"/>
+  <dimension ref="B2:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D12"/>
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G2"/>
       <c r="O2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
+      <c r="G5" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
         <v>11.26</v>
       </c>
-      <c r="D6" s="54"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D6" s="48"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="24"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1292,12 +1363,20 @@
         <f>'Financial Model'!M19</f>
         <v>448.84823499999999</v>
       </c>
-      <c r="D7" s="54" t="str">
+      <c r="D7" s="48" t="str">
         <f>$C$26</f>
         <v>Q322</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G7" s="27"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="24"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1305,250 +1384,313 @@
         <f>C6*C7</f>
         <v>5054.0311260999997</v>
       </c>
-      <c r="D8" s="54"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D8" s="48"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9">
-        <v>1964</v>
-      </c>
-      <c r="D9" s="54" t="str">
+        <f>'Financial Model'!M62</f>
+        <v>1382.6510000000001</v>
+      </c>
+      <c r="D9" s="48" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$26</f>
         <v>Q322</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G9" s="27"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="9">
-        <v>1250.4000000000001</v>
-      </c>
-      <c r="D10" s="54" t="str">
+        <f>'Financial Model'!M63</f>
+        <v>1250.434</v>
+      </c>
+      <c r="D10" s="48" t="str">
         <f t="shared" si="0"/>
         <v>Q322</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="25"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G10" s="27"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="9">
         <f>C9-C10</f>
-        <v>713.59999999999991</v>
-      </c>
-      <c r="D11" s="54" t="str">
+        <v>132.2170000000001</v>
+      </c>
+      <c r="D11" s="48" t="str">
         <f t="shared" si="0"/>
         <v>Q322</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="25"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G11" s="27"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="10">
         <f>C8-C11</f>
-        <v>4340.4311261000003</v>
-      </c>
-      <c r="D12" s="55"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="25"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G13" s="28"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G14" s="28"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="25"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="42" t="s">
+        <v>4921.8141261000001</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="G12" s="36">
+        <v>43922</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G13" s="27"/>
+      <c r="H13" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G14" s="27"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="24"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B15" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="G15" s="36">
+        <v>42917</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="54"/>
+      <c r="E16" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="26"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B17" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="37">
-        <v>43922</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="D17" s="54"/>
+      <c r="E17" s="38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B18" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="25"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G19" s="37">
-        <v>42917</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="25"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G20" s="13"/>
-      <c r="H20" s="38" t="s">
+      <c r="D18" s="58"/>
+      <c r="E18" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="42" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B21" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="53">
         <v>2011</v>
       </c>
-      <c r="D22" s="46"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D22" s="54"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="46"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D23" s="54"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B24" s="12"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B25" s="12"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B26" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="51">
+        <v>103</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="47">
         <v>44869</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B27" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="53"/>
+      <c r="D27" s="56"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B30" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="51"/>
+      <c r="D30" s="52"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B31" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="59">
+        <f>C6/'Financial Model'!M60</f>
+        <v>6.1495261658658373</v>
+      </c>
+      <c r="D31" s="60"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B32" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="59">
+        <f>C8/SUM('Financial Model'!J3:M3)</f>
+        <v>2.7191902555775602</v>
+      </c>
+      <c r="D32" s="60"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B33" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="59">
+        <f>C12/SUM('Financial Model'!J3:M3)</f>
+        <v>2.6480543307976259</v>
+      </c>
+      <c r="D33" s="60"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B34" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="59">
+        <f>C6/SUM('Financial Model'!J18:M18)</f>
+        <v>-3.3401558260378503</v>
+      </c>
+      <c r="D34" s="60"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B35" s="12"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B36" s="12"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B37" s="13"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="G9:L9"/>
+  <mergeCells count="15">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C27:D27"/>
@@ -1569,47 +1711,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A655EE-BBAA-4073-9AD9-319B2BFB7D31}">
-  <dimension ref="A1:AD57"/>
+  <dimension ref="A1:AD73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M31" sqref="M31:M32"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.85546875" style="1" customWidth="1"/>
-    <col min="8" max="11" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" style="1"/>
-    <col min="17" max="19" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.83203125" style="1" customWidth="1"/>
+    <col min="8" max="11" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.1640625" style="1"/>
+    <col min="17" max="19" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>12</v>
@@ -1626,59 +1768,59 @@
       <c r="K1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="Q1" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="30" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AA1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AB1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AC1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AD1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="14"/>
       <c r="C2" s="16">
@@ -1708,8 +1850,8 @@
       <c r="K2" s="16">
         <v>44651</v>
       </c>
-      <c r="L2" s="32" t="s">
-        <v>69</v>
+      <c r="L2" s="16">
+        <v>44742</v>
       </c>
       <c r="M2" s="16">
         <v>44834</v>
@@ -1723,11 +1865,11 @@
       <c r="S2" s="16">
         <v>44561</v>
       </c>
-      <c r="T2" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T2" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
@@ -1756,7 +1898,9 @@
       <c r="K3" s="17">
         <v>417.20499999999998</v>
       </c>
-      <c r="L3" s="33"/>
+      <c r="L3" s="17">
+        <v>466.185</v>
+      </c>
       <c r="M3" s="17">
         <v>501.93799999999999</v>
       </c>
@@ -1769,9 +1913,9 @@
       <c r="S3" s="17">
         <v>1296.0250000000001</v>
       </c>
-      <c r="T3" s="33"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="T3" s="32"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1799,6 +1943,9 @@
       <c r="K4" s="18">
         <v>313.37900000000002</v>
       </c>
+      <c r="L4" s="18">
+        <v>312.767</v>
+      </c>
       <c r="M4" s="18">
         <v>372.69200000000001</v>
       </c>
@@ -1812,7 +1959,7 @@
         <v>794.16200000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -1847,7 +1994,10 @@
         <f>K3-K4</f>
         <v>103.82599999999996</v>
       </c>
-      <c r="L5" s="33"/>
+      <c r="L5" s="17">
+        <f>L3-L4</f>
+        <v>153.41800000000001</v>
+      </c>
       <c r="M5" s="17">
         <f>M3-M4</f>
         <v>129.24599999999998</v>
@@ -1864,9 +2014,9 @@
         <f t="shared" si="0"/>
         <v>501.86300000000006</v>
       </c>
-      <c r="T5" s="33"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="T5" s="32"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1894,6 +2044,9 @@
       <c r="K6" s="18">
         <v>321.452</v>
       </c>
+      <c r="L6" s="18">
+        <v>197.529</v>
+      </c>
       <c r="M6" s="18">
         <v>321.714</v>
       </c>
@@ -1907,7 +2060,7 @@
         <v>981.5</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1935,6 +2088,9 @@
       <c r="K7" s="18">
         <v>81.352000000000004</v>
       </c>
+      <c r="L7" s="18">
+        <v>77.201999999999998</v>
+      </c>
       <c r="M7" s="18">
         <v>76.299000000000007</v>
       </c>
@@ -1948,7 +2104,7 @@
         <v>253.655</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1976,6 +2132,9 @@
       <c r="K8" s="18">
         <v>216.60599999999999</v>
       </c>
+      <c r="L8" s="18">
+        <v>187.60900000000001</v>
+      </c>
       <c r="M8" s="18">
         <v>186.261</v>
       </c>
@@ -1989,7 +2148,7 @@
         <v>828.32500000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2023,6 +2182,10 @@
         <f>SUM(K6:K8)</f>
         <v>619.41</v>
       </c>
+      <c r="L9" s="18">
+        <f t="shared" ref="L9" si="1">SUM(L6:L8)</f>
+        <v>462.34000000000003</v>
+      </c>
       <c r="M9" s="18">
         <f>SUM(M6:M8)</f>
         <v>584.274</v>
@@ -2040,7 +2203,7 @@
         <v>2063.48</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
@@ -2075,7 +2238,10 @@
         <f>K5-K9</f>
         <v>-515.58400000000006</v>
       </c>
-      <c r="L10" s="33"/>
+      <c r="L10" s="17">
+        <f t="shared" ref="L10" si="2">L5-L9</f>
+        <v>-308.92200000000003</v>
+      </c>
       <c r="M10" s="17">
         <f>M5-M9</f>
         <v>-455.02800000000002</v>
@@ -2092,9 +2258,9 @@
         <f>S5-S9</f>
         <v>-1561.617</v>
       </c>
-      <c r="T10" s="33"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="T10" s="32"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -2122,6 +2288,9 @@
       <c r="K11" s="18">
         <v>0.14799999999999999</v>
       </c>
+      <c r="L11" s="18">
+        <v>1.929</v>
+      </c>
       <c r="M11" s="18">
         <v>6.3010000000000002</v>
       </c>
@@ -2135,12 +2304,12 @@
         <v>1.9570000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34">
         <v>-363.36099999999999</v>
       </c>
       <c r="E12" s="18">
@@ -2157,12 +2326,15 @@
         <v>7.0910000000000002</v>
       </c>
       <c r="J12" s="18">
-        <f t="shared" ref="J12:J16" si="1">S12-I12-H12-G12</f>
+        <f t="shared" ref="J12:J16" si="3">S12-I12-H12-G12</f>
         <v>32.97</v>
       </c>
       <c r="K12" s="18">
         <v>12.680999999999999</v>
       </c>
+      <c r="L12" s="18">
+        <v>14.315</v>
+      </c>
       <c r="M12" s="18">
         <v>6.7969999999999997</v>
       </c>
@@ -2176,7 +2348,7 @@
         <v>30.065000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
@@ -2198,12 +2370,15 @@
         <v>0</v>
       </c>
       <c r="J13" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.951000000000001</v>
       </c>
       <c r="K13" s="18">
         <v>37.881999999999998</v>
       </c>
+      <c r="L13" s="18">
+        <v>-5.5730000000000004</v>
+      </c>
       <c r="M13" s="18">
         <v>8.2569999999999997</v>
       </c>
@@ -2217,7 +2392,7 @@
         <v>11.951000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2251,6 +2426,10 @@
         <f>K10+K11+K12+K13</f>
         <v>-464.87300000000005</v>
       </c>
+      <c r="L14" s="18">
+        <f>L10+L11+L12+L13</f>
+        <v>-298.25100000000003</v>
+      </c>
       <c r="M14" s="18">
         <f>M10+M11+M12+M13</f>
         <v>-433.673</v>
@@ -2268,7 +2447,7 @@
         <v>-1517.6439999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -2290,12 +2469,15 @@
         <v>3.8450000000000002</v>
       </c>
       <c r="J15" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2.5750000000000002</v>
       </c>
       <c r="K15" s="18">
         <v>0.46899999999999997</v>
       </c>
+      <c r="L15" s="18">
+        <v>-81.225999999999999</v>
+      </c>
       <c r="M15" s="18">
         <v>3.177</v>
       </c>
@@ -2309,7 +2491,7 @@
         <v>8.2690000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
@@ -2331,12 +2513,15 @@
         <v>0.20200000000000001</v>
       </c>
       <c r="J16" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-3.2669999999999999</v>
       </c>
       <c r="K16" s="18">
         <v>2.351</v>
       </c>
+      <c r="L16" s="18">
+        <v>7.8E-2</v>
+      </c>
       <c r="M16" s="18">
         <v>0.05</v>
       </c>
@@ -2350,7 +2535,7 @@
         <v>-2.718</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>38</v>
@@ -2385,7 +2570,10 @@
         <f>K14-K15-K16</f>
         <v>-467.69300000000004</v>
       </c>
-      <c r="L17" s="33"/>
+      <c r="L17" s="17">
+        <f>L14-L15-L16</f>
+        <v>-217.10300000000004</v>
+      </c>
       <c r="M17" s="17">
         <f>M14-M15-M16</f>
         <v>-436.90000000000003</v>
@@ -2402,72 +2590,93 @@
         <f>S14-S15-S16</f>
         <v>-1523.1949999999997</v>
       </c>
-      <c r="T17" s="33"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T17" s="32"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20">
         <f>D17/D19</f>
         <v>-1.7973026658264608</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <f>E17/E19</f>
         <v>-1.1117195841528522</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21">
+      <c r="F18" s="20"/>
+      <c r="G18" s="20">
         <f>G17/G19</f>
         <v>-0.89415297481772871</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="20">
         <f>H17/H19</f>
         <v>-0.76106185872605847</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="20">
         <f>I17/I19</f>
         <v>-1.3496003407256272</v>
+      </c>
+      <c r="J18" s="20">
+        <f>J17/J19</f>
+        <v>-0.7759483101906044</v>
       </c>
       <c r="K18" s="20">
         <f>K17/K19</f>
         <v>-1.1377564673312803</v>
       </c>
-      <c r="M18" s="21">
-        <f>M19/M17</f>
-        <v>-1.027347756923781</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="35" t="s">
+      <c r="L18" s="20">
+        <f>L17/L19</f>
+        <v>-0.48401519653842118</v>
+      </c>
+      <c r="M18" s="20">
+        <f>M17/M19</f>
+        <v>-0.97338023396705575</v>
+      </c>
+      <c r="S18" s="20">
+        <f>S17/S19</f>
+        <v>-3.7271980320231908</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="34">
         <v>291.99200000000002</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="34">
         <v>355.9</v>
       </c>
-      <c r="G19" s="35">
+      <c r="G19" s="34">
         <v>397.62099999999998</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H19" s="34">
         <v>401.447</v>
       </c>
-      <c r="I19" s="35">
+      <c r="I19" s="34">
         <v>403.84399999999999</v>
       </c>
-      <c r="K19" s="35">
+      <c r="J19" s="34">
+        <v>408.67026299999998</v>
+      </c>
+      <c r="K19" s="34">
         <v>411.06599999999997</v>
       </c>
-      <c r="L19" s="50"/>
-      <c r="M19" s="35">
+      <c r="L19" s="34">
+        <v>448.54583400000001</v>
+      </c>
+      <c r="M19" s="34">
         <v>448.84823499999999</v>
       </c>
-      <c r="T19" s="50"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S19" s="34">
+        <f>J19</f>
+        <v>408.67026299999998</v>
+      </c>
+      <c r="T19" s="46"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
@@ -2501,6 +2710,10 @@
         <f>K5/K3</f>
         <v>0.24886087175369415</v>
       </c>
+      <c r="L21" s="19">
+        <f t="shared" ref="L21" si="4">L5/L3</f>
+        <v>0.32909252764460462</v>
+      </c>
       <c r="M21" s="19">
         <f>M5/M3</f>
         <v>0.25749395343648018</v>
@@ -2510,15 +2723,15 @@
         <v>0.67876998237531305</v>
       </c>
       <c r="R21" s="19">
-        <f t="shared" ref="R21:S21" si="2">R5/R3</f>
+        <f t="shared" ref="R21:S21" si="5">R5/R3</f>
         <v>0.43601146889014736</v>
       </c>
       <c r="S21" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.38723249937308307</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
@@ -2552,6 +2765,10 @@
         <f>K10/K3</f>
         <v>-1.2358049400174975</v>
       </c>
+      <c r="L22" s="19">
+        <f t="shared" ref="L22" si="6">L10/L3</f>
+        <v>-0.66265967373467616</v>
+      </c>
       <c r="M22" s="19">
         <f>M10/M3</f>
         <v>-0.90654224226896551</v>
@@ -2561,15 +2778,15 @@
         <v>-0.45312451686713462</v>
       </c>
       <c r="R22" s="19">
-        <f t="shared" ref="R22:S22" si="3">R10/R3</f>
+        <f t="shared" ref="R22:S22" si="7">R10/R3</f>
         <v>-1.3721921722546588</v>
       </c>
       <c r="S22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.2049281456762022</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
@@ -2603,6 +2820,10 @@
         <f>K17/K3</f>
         <v>-1.1210148488153306</v>
       </c>
+      <c r="L23" s="19">
+        <f t="shared" ref="L23" si="8">L17/L3</f>
+        <v>-0.46570138464343563</v>
+      </c>
       <c r="M23" s="19">
         <f>M17/M3</f>
         <v>-0.87042622794050273</v>
@@ -2612,15 +2833,15 @@
         <v>-0.44134071302680805</v>
       </c>
       <c r="R23" s="19">
-        <f t="shared" ref="R23:S23" si="4">R17/R3</f>
+        <f t="shared" ref="R23:S23" si="9">R17/R3</f>
         <v>-2.0045091223890701</v>
       </c>
       <c r="S23" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-1.1752821126135682</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
@@ -2630,82 +2851,89 @@
         <v>-6.1595025105216884E-4</v>
       </c>
       <c r="E24" s="19">
-        <f t="shared" ref="E24:K24" si="5">E15/E14</f>
+        <f t="shared" ref="E24:K24" si="10">E15/E14</f>
         <v>3.2863220747309633E-5</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-1.3099154470246814E-2</v>
       </c>
       <c r="H24" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-7.9358791528019862E-3</v>
       </c>
       <c r="I24" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-7.107458487451499E-3</v>
       </c>
       <c r="J24" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>7.9733951800439115E-3</v>
       </c>
       <c r="K24" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-1.0088776934775734E-3</v>
       </c>
+      <c r="L24" s="19">
+        <f t="shared" ref="L24" si="11">L15/L14</f>
+        <v>0.27234108184046318</v>
+      </c>
       <c r="M24" s="19">
-        <f t="shared" ref="M24" si="6">M15/M14</f>
+        <f t="shared" ref="M24" si="12">M15/M14</f>
         <v>-7.3257961643911429E-3</v>
       </c>
       <c r="Q24" s="19">
-        <f t="shared" ref="Q24:S24" si="7">Q15/Q14</f>
+        <f t="shared" ref="Q24:S24" si="13">Q15/Q14</f>
         <v>-4.0788483582635362E-4</v>
       </c>
       <c r="R24" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>5.0491480171541148E-4</v>
       </c>
       <c r="S24" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>-5.4485768731006752E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="21">
         <f>I3/E3-1</f>
         <v>0.60211840163810981</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22">
+      <c r="J26" s="21"/>
+      <c r="K26" s="21">
         <f>K3/G3-1</f>
         <v>0.33601365458760823</v>
       </c>
-      <c r="L26" s="33"/>
-      <c r="M26" s="22">
+      <c r="L26" s="21">
+        <f>L3/H3-1</f>
+        <v>0.5664555367013322</v>
+      </c>
+      <c r="M26" s="21">
         <f>M3/I3-1</f>
         <v>1.3585206208092324</v>
       </c>
-      <c r="Q26" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="R26" s="22">
+      <c r="Q26" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="R26" s="21">
         <f>R3/Q3-1</f>
         <v>0.90016387866794467</v>
       </c>
-      <c r="S26" s="22">
-        <f t="shared" ref="S26" si="8">S3/R3-1</f>
+      <c r="S26" s="21">
+        <f t="shared" ref="S26" si="14">S3/R3-1</f>
         <v>1.1089625926721474</v>
       </c>
-      <c r="T26" s="33"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T26" s="32"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E27" s="19">
         <f>E3/D3-1</f>
@@ -2723,22 +2951,34 @@
         <f>J3/I3-1</f>
         <v>1.2240730385914795</v>
       </c>
-      <c r="Q27" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="R27" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="S27" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K27" s="19">
+        <f t="shared" ref="K27:M27" si="15">K3/J3-1</f>
+        <v>-0.11856546770189635</v>
+      </c>
+      <c r="L27" s="19">
+        <f t="shared" si="15"/>
+        <v>0.11740031878812585</v>
+      </c>
+      <c r="M27" s="19">
+        <f t="shared" si="15"/>
+        <v>7.6692729281293781E-2</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="S27" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B30" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="3" t="s">
         <v>6</v>
@@ -2762,7 +3002,9 @@
       <c r="K31" s="17">
         <v>1772.8920000000001</v>
       </c>
-      <c r="L31" s="33"/>
+      <c r="L31" s="17">
+        <v>1514.3710000000001</v>
+      </c>
       <c r="M31" s="17">
         <v>1382.6510000000001</v>
       </c>
@@ -2774,12 +3016,12 @@
         <f>K31</f>
         <v>1772.8920000000001</v>
       </c>
-      <c r="T31" s="33"/>
-    </row>
-    <row r="32" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T31" s="32"/>
+    </row>
+    <row r="32" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -2800,24 +3042,26 @@
       <c r="K32" s="17">
         <v>464.85399999999998</v>
       </c>
-      <c r="L32" s="33"/>
+      <c r="L32" s="17">
+        <v>426.16899999999998</v>
+      </c>
       <c r="M32" s="17">
         <v>581.35500000000002</v>
       </c>
       <c r="R32" s="17">
-        <f t="shared" ref="R32:R57" si="9">F32</f>
+        <f t="shared" ref="R32:R57" si="16">F32</f>
         <v>287.71800000000002</v>
       </c>
       <c r="S32" s="17">
-        <f t="shared" ref="S32:S57" si="10">K32</f>
+        <f t="shared" ref="S32:S57" si="17">K32</f>
         <v>464.85399999999998</v>
       </c>
-      <c r="T32" s="33"/>
-    </row>
-    <row r="33" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T32" s="32"/>
+    </row>
+    <row r="33" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -2838,23 +3082,25 @@
       <c r="K33" s="17">
         <v>55.945999999999998</v>
       </c>
-      <c r="L33" s="33"/>
+      <c r="L33" s="17">
+        <v>56.82</v>
+      </c>
       <c r="M33" s="17">
         <v>89.453999999999994</v>
       </c>
       <c r="R33" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>30.248999999999999</v>
       </c>
       <c r="S33" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>55.945999999999998</v>
       </c>
-      <c r="T33" s="33"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T33" s="32"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -2875,21 +3121,24 @@
       <c r="K34" s="18">
         <v>48.210999999999999</v>
       </c>
+      <c r="L34" s="18">
+        <v>45.06</v>
+      </c>
       <c r="M34" s="18">
         <v>40.991</v>
       </c>
       <c r="R34" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>44.521999999999998</v>
       </c>
       <c r="S34" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>48.210999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
@@ -2910,62 +3159,69 @@
       <c r="K35" s="18">
         <v>56.561999999999998</v>
       </c>
+      <c r="L35" s="18">
+        <v>95.248999999999995</v>
+      </c>
       <c r="M35" s="18">
         <v>98.626999999999995</v>
       </c>
       <c r="R35" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>14.558</v>
       </c>
       <c r="S35" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>56.561999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18">
-        <f t="shared" ref="F36:J36" si="11">SUM(F31:F35)</f>
+        <f t="shared" ref="F36:J36" si="18">SUM(F31:F35)</f>
         <v>2194.3049999999998</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>3056.9639999999999</v>
       </c>
       <c r="I36" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>2985.0720000000001</v>
       </c>
       <c r="J36" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>2753.33</v>
       </c>
       <c r="K36" s="18">
         <f>SUM(K31:K35)</f>
         <v>2398.4649999999997</v>
       </c>
+      <c r="L36" s="18">
+        <f>SUM(L31:L35)</f>
+        <v>2137.6689999999999</v>
+      </c>
       <c r="M36" s="18">
         <f>SUM(M31:M35)</f>
         <v>2193.078</v>
       </c>
       <c r="R36" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2194.3049999999998</v>
       </c>
       <c r="S36" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2398.4649999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -2986,21 +3242,24 @@
       <c r="K37" s="18">
         <v>49.734000000000002</v>
       </c>
+      <c r="L37" s="18">
+        <v>53.926000000000002</v>
+      </c>
       <c r="M37" s="18">
         <v>58.225999999999999</v>
       </c>
       <c r="R37" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>40.826999999999998</v>
       </c>
       <c r="S37" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>49.734000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -3026,22 +3285,26 @@
         <f>523.023+615.655</f>
         <v>1138.6779999999999</v>
       </c>
+      <c r="L38" s="18">
+        <f>810.525+894.019</f>
+        <v>1704.5439999999999</v>
+      </c>
       <c r="M38" s="18">
         <f>788.647+894.019</f>
         <v>1682.6660000000002</v>
       </c>
       <c r="R38" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>1125.5329999999999</v>
       </c>
       <c r="S38" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>1138.6779999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -3063,21 +3326,24 @@
       <c r="K39" s="18">
         <v>61.168999999999997</v>
       </c>
+      <c r="L39" s="18">
+        <v>77.337999999999994</v>
+      </c>
       <c r="M39" s="18">
         <v>74.703000000000003</v>
       </c>
       <c r="R39" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>68.076999999999998</v>
       </c>
       <c r="S39" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>61.168999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -3098,21 +3364,24 @@
       <c r="K40" s="18">
         <v>7.4740000000000002</v>
       </c>
+      <c r="L40" s="18">
+        <v>8.7959999999999994</v>
+      </c>
       <c r="M40" s="18">
         <v>8.7460000000000004</v>
       </c>
       <c r="R40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2.9550000000000001</v>
       </c>
       <c r="S40" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>7.4740000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -3133,62 +3402,68 @@
       <c r="K41" s="17">
         <v>90.795000000000002</v>
       </c>
-      <c r="L41" s="33"/>
+      <c r="L41" s="17">
+        <v>171.49100000000001</v>
+      </c>
       <c r="M41" s="17">
         <v>174.63399999999999</v>
       </c>
       <c r="R41" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>7.6319999999999997</v>
       </c>
       <c r="S41" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>90.795000000000002</v>
       </c>
-      <c r="T41" s="33"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T41" s="32"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18">
-        <f t="shared" ref="F42" si="12">F36+SUM(F37:F41)</f>
+        <f t="shared" ref="F42" si="19">F36+SUM(F37:F41)</f>
         <v>3439.3289999999997</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="18">
-        <f t="shared" ref="H42:J42" si="13">H36+SUM(H37:H41)</f>
+        <f t="shared" ref="H42:J42" si="20">H36+SUM(H37:H41)</f>
         <v>4358.8559999999998</v>
       </c>
       <c r="I42" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>4259.4210000000003</v>
       </c>
       <c r="J42" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>4069.0540000000001</v>
       </c>
       <c r="K42" s="18">
         <f>K36+SUM(K37:K41)</f>
         <v>3746.3149999999996</v>
       </c>
+      <c r="L42" s="18">
+        <f>L36+SUM(L37:L41)</f>
+        <v>4153.7639999999992</v>
+      </c>
       <c r="M42" s="18">
         <f>M36+SUM(M37:M41)</f>
         <v>4192.0529999999999</v>
       </c>
       <c r="R42" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>3439.3289999999997</v>
       </c>
       <c r="S42" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>3746.3149999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
@@ -3202,9 +3477,9 @@
       <c r="R43" s="18"/>
       <c r="S43" s="17"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -3225,21 +3500,24 @@
       <c r="K44" s="18">
         <v>379.25400000000002</v>
       </c>
+      <c r="L44" s="18">
+        <v>414.68</v>
+      </c>
       <c r="M44" s="18">
         <v>560.79399999999998</v>
       </c>
       <c r="R44" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>223.63300000000001</v>
       </c>
       <c r="S44" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>379.25400000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -3260,21 +3538,24 @@
       <c r="K45" s="18">
         <v>520.77499999999998</v>
       </c>
+      <c r="L45" s="18">
+        <v>482.94</v>
+      </c>
       <c r="M45" s="18">
         <v>670.78399999999999</v>
       </c>
       <c r="R45" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>317.94200000000001</v>
       </c>
       <c r="S45" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>520.77499999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -3295,21 +3576,24 @@
       <c r="K46" s="18">
         <v>12.911</v>
       </c>
+      <c r="L46" s="18">
+        <v>5.726</v>
+      </c>
       <c r="M46" s="18">
         <v>5.6449999999999996</v>
       </c>
       <c r="R46" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>12.837</v>
       </c>
       <c r="S46" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>12.911</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -3332,22 +3616,25 @@
       <c r="K47" s="18">
         <v>0</v>
       </c>
+      <c r="L47" s="18">
+        <v>17.283000000000001</v>
+      </c>
       <c r="M47" s="18">
         <v>47.951000000000001</v>
       </c>
       <c r="R47" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S47" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="B48" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -3373,23 +3660,27 @@
         <f>SUM(K44:K47)</f>
         <v>912.93999999999994</v>
       </c>
+      <c r="L48" s="18">
+        <f>SUM(L44:L47)</f>
+        <v>920.62900000000002</v>
+      </c>
       <c r="M48" s="18">
         <f>SUM(M44:M47)</f>
         <v>1285.174</v>
       </c>
       <c r="R48" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>554.41200000000003</v>
       </c>
       <c r="S48" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>912.93999999999994</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -3410,23 +3701,25 @@
       <c r="K49" s="17">
         <v>1249.106</v>
       </c>
-      <c r="L49" s="33"/>
+      <c r="L49" s="17">
+        <v>1249.7660000000001</v>
+      </c>
       <c r="M49" s="17">
         <v>1250.434</v>
       </c>
       <c r="R49" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S49" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>1249.106</v>
       </c>
-      <c r="T49" s="33"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T49" s="32"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
@@ -3447,21 +3740,24 @@
       <c r="K50" s="18">
         <v>54.457000000000001</v>
       </c>
+      <c r="L50" s="18">
+        <v>78.176000000000002</v>
+      </c>
       <c r="M50" s="18">
         <v>76.08</v>
       </c>
       <c r="R50" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>68.775000000000006</v>
       </c>
       <c r="S50" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>54.457000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
@@ -3482,21 +3778,24 @@
       <c r="K51" s="18">
         <v>14.23</v>
       </c>
+      <c r="L51" s="18">
+        <v>13.081</v>
+      </c>
       <c r="M51" s="18">
         <v>19.876999999999999</v>
       </c>
       <c r="R51" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>65.444000000000003</v>
       </c>
       <c r="S51" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>14.23</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -3517,21 +3816,24 @@
       <c r="K52" s="18">
         <v>78.947000000000003</v>
       </c>
+      <c r="L52" s="18">
+        <v>73.858999999999995</v>
+      </c>
       <c r="M52" s="18">
         <v>67.924999999999997</v>
       </c>
       <c r="R52" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>72.066000000000003</v>
       </c>
       <c r="S52" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>78.947000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -3552,60 +3854,67 @@
       <c r="K53" s="18">
         <v>51.034999999999997</v>
       </c>
+      <c r="L53" s="18">
+        <v>54.369</v>
+      </c>
       <c r="M53" s="18">
         <v>57.447000000000003</v>
       </c>
       <c r="R53" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>47.286999999999999</v>
       </c>
       <c r="S53" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>51.034999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18">
-        <f t="shared" ref="F54" si="14">F48+SUM(F49:F53)</f>
+        <f t="shared" ref="F54" si="21">F48+SUM(F49:F53)</f>
         <v>807.98400000000004</v>
       </c>
       <c r="G54" s="18"/>
       <c r="H54" s="18">
-        <f t="shared" ref="H54:J54" si="15">H48+SUM(H49:H53)</f>
+        <f t="shared" ref="H54:J54" si="22">H48+SUM(H49:H53)</f>
         <v>2153.5039999999999</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>2432.8900000000003</v>
       </c>
       <c r="J54" s="18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>2390.5259999999998</v>
       </c>
       <c r="K54" s="18">
         <f>K48+SUM(K49:K53)</f>
         <v>2360.7150000000001</v>
       </c>
+      <c r="L54" s="18">
+        <f>L48+SUM(L49:L53)</f>
+        <v>2389.8799999999997</v>
+      </c>
       <c r="M54" s="18">
         <f>M48+SUM(M49:M53)</f>
         <v>2756.9369999999999</v>
       </c>
       <c r="R54" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>807.98400000000004</v>
       </c>
       <c r="S54" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2360.7150000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A55" s="3"/>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -3618,17 +3927,17 @@
       <c r="K55" s="18"/>
       <c r="M55" s="18"/>
       <c r="R55" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S55" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -3649,6 +3958,9 @@
       <c r="K56" s="18">
         <v>1385.6</v>
       </c>
+      <c r="L56" s="18">
+        <v>1763.884</v>
+      </c>
       <c r="M56" s="18">
         <v>1435.116</v>
       </c>
@@ -3657,49 +3969,463 @@
         <v>2631.3449999999998</v>
       </c>
       <c r="S56" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>1385.6</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18">
-        <f t="shared" ref="F57" si="16">F56+F54</f>
+        <f t="shared" ref="F57" si="23">F56+F54</f>
         <v>3439.3289999999997</v>
       </c>
       <c r="G57" s="18"/>
       <c r="H57" s="18">
-        <f t="shared" ref="H57:J57" si="17">H56+H54</f>
+        <f t="shared" ref="H57:J57" si="24">H56+H54</f>
         <v>4358.8559999999998</v>
       </c>
       <c r="I57" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>4259.0570000000007</v>
       </c>
       <c r="J57" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>4069.0540000000001</v>
       </c>
       <c r="K57" s="18">
         <f>K56+K54</f>
         <v>3746.3150000000001</v>
       </c>
+      <c r="L57" s="18">
+        <f>L56+L54</f>
+        <v>4153.7639999999992</v>
+      </c>
       <c r="M57" s="18">
         <f>M56+M54</f>
         <v>4192.0529999999999</v>
       </c>
       <c r="R57" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>3439.3289999999997</v>
       </c>
       <c r="S57" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>3746.3150000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H59" s="18">
+        <f t="shared" ref="H59:M59" si="25">H31-H44</f>
+        <v>2351.904</v>
+      </c>
+      <c r="I59" s="18">
+        <f t="shared" si="25"/>
+        <v>1978.3279999999997</v>
+      </c>
+      <c r="J59" s="18">
+        <f t="shared" si="25"/>
+        <v>1765.1549999999997</v>
+      </c>
+      <c r="K59" s="18">
+        <f t="shared" si="25"/>
+        <v>1393.6379999999999</v>
+      </c>
+      <c r="L59" s="18">
+        <f t="shared" si="25"/>
+        <v>1099.691</v>
+      </c>
+      <c r="M59" s="18">
+        <f>M31-M44</f>
+        <v>821.85700000000008</v>
+      </c>
+      <c r="R59" s="18">
+        <f>R31-R44</f>
+        <v>1593.625</v>
+      </c>
+      <c r="S59" s="18">
+        <f>S31-S44</f>
+        <v>1393.6379999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" ref="H60:L60" si="26">H59/H19</f>
+        <v>5.8585666351971746</v>
+      </c>
+      <c r="I60" s="1">
+        <f t="shared" si="26"/>
+        <v>4.8987430790107069</v>
+      </c>
+      <c r="J60" s="1">
+        <f t="shared" si="26"/>
+        <v>4.3192645998811026</v>
+      </c>
+      <c r="K60" s="1">
+        <f t="shared" si="26"/>
+        <v>3.3903022872239497</v>
+      </c>
+      <c r="L60" s="1">
+        <f t="shared" si="26"/>
+        <v>2.4516803337426607</v>
+      </c>
+      <c r="M60" s="1">
+        <f>M59/M19</f>
+        <v>1.8310353832626747</v>
+      </c>
+      <c r="R60" s="1" t="e">
+        <f>R59/R19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S60" s="1">
+        <f>S59/S19</f>
+        <v>3.4101771676986443</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H62" s="18">
+        <f t="shared" ref="H62:M62" si="27">H31</f>
+        <v>2646.5</v>
+      </c>
+      <c r="I62" s="18">
+        <f t="shared" si="27"/>
+        <v>2394.8649999999998</v>
+      </c>
+      <c r="J62" s="18">
+        <f t="shared" si="27"/>
+        <v>2152.8919999999998</v>
+      </c>
+      <c r="K62" s="18">
+        <f t="shared" si="27"/>
+        <v>1772.8920000000001</v>
+      </c>
+      <c r="L62" s="18">
+        <f t="shared" si="27"/>
+        <v>1514.3710000000001</v>
+      </c>
+      <c r="M62" s="18">
+        <f>M31</f>
+        <v>1382.6510000000001</v>
+      </c>
+      <c r="R62" s="18">
+        <f>R31</f>
+        <v>1817.258</v>
+      </c>
+      <c r="S62" s="18">
+        <f>S31</f>
+        <v>1772.8920000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="18">
+        <f t="shared" ref="H63:M63" si="28">H49</f>
+        <v>1247.1179999999999</v>
+      </c>
+      <c r="I63" s="18">
+        <f t="shared" si="28"/>
+        <v>1247.7850000000001</v>
+      </c>
+      <c r="J63" s="18">
+        <f t="shared" si="28"/>
+        <v>1248.452</v>
+      </c>
+      <c r="K63" s="18">
+        <f t="shared" si="28"/>
+        <v>1249.106</v>
+      </c>
+      <c r="L63" s="18">
+        <f t="shared" si="28"/>
+        <v>1249.7660000000001</v>
+      </c>
+      <c r="M63" s="18">
+        <f>M49</f>
+        <v>1250.434</v>
+      </c>
+      <c r="R63" s="18">
+        <f>R49</f>
+        <v>0</v>
+      </c>
+      <c r="S63" s="18">
+        <f>S49</f>
+        <v>1249.106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="18">
+        <f t="shared" ref="H64:L64" si="29">H62-H63</f>
+        <v>1399.3820000000001</v>
+      </c>
+      <c r="I64" s="18">
+        <f t="shared" si="29"/>
+        <v>1147.0799999999997</v>
+      </c>
+      <c r="J64" s="18">
+        <f t="shared" si="29"/>
+        <v>904.43999999999983</v>
+      </c>
+      <c r="K64" s="18">
+        <f t="shared" si="29"/>
+        <v>523.78600000000006</v>
+      </c>
+      <c r="L64" s="18">
+        <f t="shared" si="29"/>
+        <v>264.60500000000002</v>
+      </c>
+      <c r="M64" s="18">
+        <f>M62-M63</f>
+        <v>132.2170000000001</v>
+      </c>
+      <c r="R64" s="18">
+        <f>R62-R63</f>
+        <v>1817.258</v>
+      </c>
+      <c r="S64" s="18">
+        <f>S62-S63</f>
+        <v>523.78600000000006</v>
+      </c>
+    </row>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F66" s="1">
+        <v>46.56</v>
+      </c>
+      <c r="H66" s="1">
+        <v>52.17</v>
+      </c>
+      <c r="I66" s="1">
+        <v>48.16</v>
+      </c>
+      <c r="J66" s="1">
+        <v>27.47</v>
+      </c>
+      <c r="K66" s="1">
+        <v>19.47</v>
+      </c>
+      <c r="L66" s="1">
+        <v>11.67</v>
+      </c>
+      <c r="M66" s="1">
+        <v>15.14</v>
+      </c>
+      <c r="R66" s="1">
+        <v>15.14</v>
+      </c>
+      <c r="S66" s="1">
+        <v>15.14</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="18">
+        <f t="shared" ref="F67:L67" si="30">F66*F19</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="18">
+        <f t="shared" si="30"/>
+        <v>20943.489990000002</v>
+      </c>
+      <c r="I67" s="18">
+        <f t="shared" si="30"/>
+        <v>19449.127039999999</v>
+      </c>
+      <c r="J67" s="18">
+        <f t="shared" si="30"/>
+        <v>11226.172124609999</v>
+      </c>
+      <c r="K67" s="18">
+        <f t="shared" si="30"/>
+        <v>8003.4550199999994</v>
+      </c>
+      <c r="L67" s="18">
+        <f t="shared" si="30"/>
+        <v>5234.5298827799998</v>
+      </c>
+      <c r="M67" s="18">
+        <f>M66*M19</f>
+        <v>6795.5622779000005</v>
+      </c>
+      <c r="R67" s="18">
+        <f>R66*R19</f>
+        <v>0</v>
+      </c>
+      <c r="S67" s="18">
+        <f>S66*S19</f>
+        <v>6187.26778182</v>
+      </c>
+    </row>
+    <row r="68" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="18">
+        <f t="shared" ref="F68:L68" si="31">F67-F64</f>
+        <v>0</v>
+      </c>
+      <c r="H68" s="18">
+        <f t="shared" si="31"/>
+        <v>19544.10799</v>
+      </c>
+      <c r="I68" s="18">
+        <f t="shared" si="31"/>
+        <v>18302.047040000001</v>
+      </c>
+      <c r="J68" s="18">
+        <f t="shared" si="31"/>
+        <v>10321.732124609998</v>
+      </c>
+      <c r="K68" s="18">
+        <f t="shared" si="31"/>
+        <v>7479.6690199999994</v>
+      </c>
+      <c r="L68" s="18">
+        <f t="shared" si="31"/>
+        <v>4969.9248827800002</v>
+      </c>
+      <c r="M68" s="18">
+        <f>M67-M64</f>
+        <v>6663.3452778999999</v>
+      </c>
+      <c r="R68" s="18">
+        <f>R67-R64</f>
+        <v>-1817.258</v>
+      </c>
+      <c r="S68" s="18">
+        <f>S67-S64</f>
+        <v>5663.4817818199999</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B70" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70" s="61"/>
+      <c r="H70" s="61">
+        <f t="shared" ref="F70:M70" si="32">H66/H60</f>
+        <v>8.9049085294297718</v>
+      </c>
+      <c r="I70" s="61">
+        <f t="shared" si="32"/>
+        <v>9.8310932464181864</v>
+      </c>
+      <c r="J70" s="61">
+        <f t="shared" si="32"/>
+        <v>6.3598789480867115</v>
+      </c>
+      <c r="K70" s="61">
+        <f t="shared" si="32"/>
+        <v>5.7428507402926723</v>
+      </c>
+      <c r="L70" s="61">
+        <f t="shared" si="32"/>
+        <v>4.7600006572573568</v>
+      </c>
+      <c r="M70" s="61">
+        <f>M66/M60</f>
+        <v>8.268545839361348</v>
+      </c>
+      <c r="S70" s="61">
+        <f>S66/S60</f>
+        <v>4.4396520343302921</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B71" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J71" s="61">
+        <f>J67/SUM(G3:J3)</f>
+        <v>8.6620027581335215</v>
+      </c>
+      <c r="K71" s="61">
+        <f>K67/SUM(H3:K3)</f>
+        <v>5.7128606792228718</v>
+      </c>
+      <c r="L71" s="61">
+        <f>L67/SUM(I3:L3)</f>
+        <v>3.3350853710591801</v>
+      </c>
+      <c r="M71" s="61">
+        <f>M67/SUM(J3:M3)</f>
+        <v>3.6561758853858142</v>
+      </c>
+      <c r="S71" s="61">
+        <f>S67/S3</f>
+        <v>4.7740342831504021</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B72" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H72" s="61"/>
+      <c r="I72" s="61"/>
+      <c r="J72" s="61">
+        <f t="shared" ref="H72:L72" si="33">J68/SUM(G3:J3)</f>
+        <v>7.964145849509074</v>
+      </c>
+      <c r="K72" s="61">
+        <f t="shared" si="33"/>
+        <v>5.3389825932900008</v>
+      </c>
+      <c r="L72" s="61">
+        <f t="shared" si="33"/>
+        <v>3.1664971149271057</v>
+      </c>
+      <c r="M72" s="61">
+        <f>M68/SUM(J3:M3)</f>
+        <v>3.5850399606058789</v>
+      </c>
+      <c r="S72" s="61">
+        <f>S68/S3</f>
+        <v>4.3698862150190001</v>
+      </c>
+    </row>
+    <row r="73" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B73" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J73" s="61">
+        <f t="shared" ref="J73:L73" si="34">J66/SUM(G18:J18)</f>
+        <v>-7.2657282352914372</v>
+      </c>
+      <c r="K73" s="61">
+        <f t="shared" si="34"/>
+        <v>-4.8380279709585396</v>
+      </c>
+      <c r="L73" s="61">
+        <f t="shared" si="34"/>
+        <v>-3.1142253716484478</v>
+      </c>
+      <c r="M73" s="61">
+        <f>M66/SUM(J18:M18)</f>
+        <v>-4.4911153824345522</v>
+      </c>
+      <c r="S73" s="61">
+        <f>S66/S18</f>
+        <v>-4.0620326234132866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct BVPS formula in $DKNG
</commit_message>
<xml_diff>
--- a/$DKNG.xlsx
+++ b/$DKNG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5421C-D4E4-7B4A-9245-4A277741C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E86AA9-ACE6-284C-BC67-317C0BA034C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18900" xr2:uid="{E77186FA-83D4-479E-A0A9-B880EBEEF096}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18900" activeTab="1" xr2:uid="{E77186FA-83D4-479E-A0A9-B880EBEEF096}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0\x"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -713,6 +713,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,13 +747,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72920D05-7E62-4C8A-A716-46BB4747797C}">
   <dimension ref="B2:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:D34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1322,21 +1322,21 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="G5" s="50" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="G5" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
@@ -1502,11 +1502,11 @@
       <c r="N14" s="24"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
       <c r="G15" s="36">
         <v>42917</v>
       </c>
@@ -1524,10 +1524,10 @@
       <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="54"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="38" t="s">
         <v>94</v>
       </c>
@@ -1546,10 +1546,10 @@
       <c r="B17" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="54"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="38" t="s">
         <v>94</v>
       </c>
@@ -1558,38 +1558,38 @@
       <c r="B18" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="58"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="38" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="53">
+      <c r="C22" s="56">
         <v>2011</v>
       </c>
-      <c r="D22" s="54"/>
+      <c r="D22" s="57"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="54"/>
+      <c r="D23" s="57"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B24" s="12"/>
@@ -1616,57 +1616,57 @@
       <c r="B27" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="59"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B31" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="59">
+      <c r="C31" s="51">
         <f>C6/'Financial Model'!M60</f>
-        <v>6.1495261658658373</v>
-      </c>
-      <c r="D31" s="60"/>
+        <v>3.5216882301500365</v>
+      </c>
+      <c r="D31" s="52"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B32" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="59">
+      <c r="C32" s="51">
         <f>C8/SUM('Financial Model'!J3:M3)</f>
         <v>2.7191902555775602</v>
       </c>
-      <c r="D32" s="60"/>
+      <c r="D32" s="52"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="59">
+      <c r="C33" s="51">
         <f>C12/SUM('Financial Model'!J3:M3)</f>
         <v>2.6480543307976259</v>
       </c>
-      <c r="D33" s="60"/>
+      <c r="D33" s="52"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="59">
+      <c r="C34" s="51">
         <f>C6/SUM('Financial Model'!J18:M18)</f>
         <v>-3.3401558260378503</v>
       </c>
-      <c r="D34" s="60"/>
+      <c r="D34" s="52"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="12"/>
@@ -1713,11 +1713,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A655EE-BBAA-4073-9AD9-319B2BFB7D31}">
   <dimension ref="A1:AD73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1975,31 +1975,31 @@
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17">
-        <f>G3-G4</f>
+        <f t="shared" ref="G5:M5" si="0">G3-G4</f>
         <v>129.05100000000002</v>
       </c>
       <c r="H5" s="17">
-        <f>H3-H4</f>
+        <f t="shared" si="0"/>
         <v>110.59900000000002</v>
       </c>
       <c r="I5" s="17">
-        <f>I3-I4</f>
+        <f t="shared" si="0"/>
         <v>42.069999999999993</v>
       </c>
       <c r="J5" s="17">
-        <f>J3-J4</f>
+        <f t="shared" si="0"/>
         <v>220.14300000000006</v>
       </c>
       <c r="K5" s="17">
-        <f>K3-K4</f>
+        <f t="shared" si="0"/>
         <v>103.82599999999996</v>
       </c>
       <c r="L5" s="17">
-        <f>L3-L4</f>
+        <f t="shared" si="0"/>
         <v>153.41800000000001</v>
       </c>
       <c r="M5" s="17">
-        <f>M3-M4</f>
+        <f t="shared" si="0"/>
         <v>129.24599999999998</v>
       </c>
       <c r="Q5" s="17">
@@ -2007,11 +2007,11 @@
         <v>219.52100000000002</v>
       </c>
       <c r="R5" s="17">
-        <f t="shared" ref="R5:S5" si="0">R3-R4</f>
+        <f t="shared" ref="R5:S5" si="1">R3-R4</f>
         <v>267.94300000000004</v>
       </c>
       <c r="S5" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>501.86300000000006</v>
       </c>
       <c r="T5" s="32"/>
@@ -2183,7 +2183,7 @@
         <v>619.41</v>
       </c>
       <c r="L9" s="18">
-        <f t="shared" ref="L9" si="1">SUM(L6:L8)</f>
+        <f t="shared" ref="L9" si="2">SUM(L6:L8)</f>
         <v>462.34000000000003</v>
       </c>
       <c r="M9" s="18">
@@ -2239,7 +2239,7 @@
         <v>-515.58400000000006</v>
       </c>
       <c r="L10" s="17">
-        <f t="shared" ref="L10" si="2">L5-L9</f>
+        <f t="shared" ref="L10" si="3">L5-L9</f>
         <v>-308.92200000000003</v>
       </c>
       <c r="M10" s="17">
@@ -2326,7 +2326,7 @@
         <v>7.0910000000000002</v>
       </c>
       <c r="J12" s="18">
-        <f t="shared" ref="J12:J16" si="3">S12-I12-H12-G12</f>
+        <f t="shared" ref="J12:J16" si="4">S12-I12-H12-G12</f>
         <v>32.97</v>
       </c>
       <c r="K12" s="18">
@@ -2370,7 +2370,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.951000000000001</v>
       </c>
       <c r="K13" s="18">
@@ -2407,31 +2407,31 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18">
-        <f>G10+G11+G12+G13</f>
+        <f t="shared" ref="G14:M14" si="5">G10+G11+G12+G13</f>
         <v>-350.78600000000006</v>
       </c>
       <c r="H14" s="18">
-        <f>H10+H11+H12+H13</f>
+        <f t="shared" si="5"/>
         <v>-302.928</v>
       </c>
       <c r="I14" s="18">
-        <f>I10+I11+I12+I13</f>
+        <f t="shared" si="5"/>
         <v>-540.98100000000011</v>
       </c>
       <c r="J14" s="18">
-        <f>J10+J11+J12+J13</f>
+        <f t="shared" si="5"/>
         <v>-322.94899999999984</v>
       </c>
       <c r="K14" s="18">
-        <f>K10+K11+K12+K13</f>
+        <f t="shared" si="5"/>
         <v>-464.87300000000005</v>
       </c>
       <c r="L14" s="18">
-        <f>L10+L11+L12+L13</f>
+        <f t="shared" si="5"/>
         <v>-298.25100000000003</v>
       </c>
       <c r="M14" s="18">
-        <f>M10+M11+M12+M13</f>
+        <f t="shared" si="5"/>
         <v>-433.673</v>
       </c>
       <c r="Q14" s="18">
@@ -2469,7 +2469,7 @@
         <v>3.8450000000000002</v>
       </c>
       <c r="J15" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.5750000000000002</v>
       </c>
       <c r="K15" s="18">
@@ -2513,7 +2513,7 @@
         <v>0.20200000000000001</v>
       </c>
       <c r="J16" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.2669999999999999</v>
       </c>
       <c r="K16" s="18">
@@ -2551,31 +2551,31 @@
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17">
-        <f>G14-G15-G16</f>
+        <f t="shared" ref="G17:M17" si="6">G14-G15-G16</f>
         <v>-355.53400000000011</v>
       </c>
       <c r="H17" s="17">
-        <f>H14-H15-H16</f>
+        <f t="shared" si="6"/>
         <v>-305.52600000000001</v>
       </c>
       <c r="I17" s="17">
-        <f>I14-I15-I16</f>
+        <f t="shared" si="6"/>
         <v>-545.02800000000013</v>
       </c>
       <c r="J17" s="17">
-        <f>J14-J15-J16</f>
+        <f t="shared" si="6"/>
         <v>-317.10699999999986</v>
       </c>
       <c r="K17" s="17">
-        <f>K14-K15-K16</f>
+        <f t="shared" si="6"/>
         <v>-467.69300000000004</v>
       </c>
       <c r="L17" s="17">
-        <f>L14-L15-L16</f>
+        <f t="shared" si="6"/>
         <v>-217.10300000000004</v>
       </c>
       <c r="M17" s="17">
-        <f>M14-M15-M16</f>
+        <f t="shared" si="6"/>
         <v>-436.90000000000003</v>
       </c>
       <c r="Q17" s="17">
@@ -2607,31 +2607,31 @@
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20">
-        <f>G17/G19</f>
+        <f t="shared" ref="G18:M18" si="7">G17/G19</f>
         <v>-0.89415297481772871</v>
       </c>
       <c r="H18" s="20">
-        <f>H17/H19</f>
+        <f t="shared" si="7"/>
         <v>-0.76106185872605847</v>
       </c>
       <c r="I18" s="20">
-        <f>I17/I19</f>
+        <f t="shared" si="7"/>
         <v>-1.3496003407256272</v>
       </c>
       <c r="J18" s="20">
-        <f>J17/J19</f>
+        <f t="shared" si="7"/>
         <v>-0.7759483101906044</v>
       </c>
       <c r="K18" s="20">
-        <f>K17/K19</f>
+        <f t="shared" si="7"/>
         <v>-1.1377564673312803</v>
       </c>
       <c r="L18" s="20">
-        <f>L17/L19</f>
+        <f t="shared" si="7"/>
         <v>-0.48401519653842118</v>
       </c>
       <c r="M18" s="20">
-        <f>M17/M19</f>
+        <f t="shared" si="7"/>
         <v>-0.97338023396705575</v>
       </c>
       <c r="S18" s="20">
@@ -2711,7 +2711,7 @@
         <v>0.24886087175369415</v>
       </c>
       <c r="L21" s="19">
-        <f t="shared" ref="L21" si="4">L5/L3</f>
+        <f t="shared" ref="L21" si="8">L5/L3</f>
         <v>0.32909252764460462</v>
       </c>
       <c r="M21" s="19">
@@ -2723,11 +2723,11 @@
         <v>0.67876998237531305</v>
       </c>
       <c r="R21" s="19">
-        <f t="shared" ref="R21:S21" si="5">R5/R3</f>
+        <f t="shared" ref="R21:S21" si="9">R5/R3</f>
         <v>0.43601146889014736</v>
       </c>
       <c r="S21" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.38723249937308307</v>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
         <v>-1.2358049400174975</v>
       </c>
       <c r="L22" s="19">
-        <f t="shared" ref="L22" si="6">L10/L3</f>
+        <f t="shared" ref="L22" si="10">L10/L3</f>
         <v>-0.66265967373467616</v>
       </c>
       <c r="M22" s="19">
@@ -2778,11 +2778,11 @@
         <v>-0.45312451686713462</v>
       </c>
       <c r="R22" s="19">
-        <f t="shared" ref="R22:S22" si="7">R10/R3</f>
+        <f t="shared" ref="R22:S22" si="11">R10/R3</f>
         <v>-1.3721921722546588</v>
       </c>
       <c r="S22" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-1.2049281456762022</v>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
         <v>-1.1210148488153306</v>
       </c>
       <c r="L23" s="19">
-        <f t="shared" ref="L23" si="8">L17/L3</f>
+        <f t="shared" ref="L23" si="12">L17/L3</f>
         <v>-0.46570138464343563</v>
       </c>
       <c r="M23" s="19">
@@ -2833,11 +2833,11 @@
         <v>-0.44134071302680805</v>
       </c>
       <c r="R23" s="19">
-        <f t="shared" ref="R23:S23" si="9">R17/R3</f>
+        <f t="shared" ref="R23:S23" si="13">R17/R3</f>
         <v>-2.0045091223890701</v>
       </c>
       <c r="S23" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-1.1752821126135682</v>
       </c>
     </row>
@@ -2851,48 +2851,48 @@
         <v>-6.1595025105216884E-4</v>
       </c>
       <c r="E24" s="19">
-        <f t="shared" ref="E24:K24" si="10">E15/E14</f>
+        <f t="shared" ref="E24:K24" si="14">E15/E14</f>
         <v>3.2863220747309633E-5</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-1.3099154470246814E-2</v>
       </c>
       <c r="H24" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-7.9358791528019862E-3</v>
       </c>
       <c r="I24" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-7.107458487451499E-3</v>
       </c>
       <c r="J24" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7.9733951800439115E-3</v>
       </c>
       <c r="K24" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-1.0088776934775734E-3</v>
       </c>
       <c r="L24" s="19">
-        <f t="shared" ref="L24" si="11">L15/L14</f>
+        <f t="shared" ref="L24" si="15">L15/L14</f>
         <v>0.27234108184046318</v>
       </c>
       <c r="M24" s="19">
-        <f t="shared" ref="M24" si="12">M15/M14</f>
+        <f t="shared" ref="M24" si="16">M15/M14</f>
         <v>-7.3257961643911429E-3</v>
       </c>
       <c r="Q24" s="19">
-        <f t="shared" ref="Q24:S24" si="13">Q15/Q14</f>
+        <f t="shared" ref="Q24:S24" si="17">Q15/Q14</f>
         <v>-4.0788483582635362E-4</v>
       </c>
       <c r="R24" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>5.0491480171541148E-4</v>
       </c>
       <c r="S24" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-5.4485768731006752E-3</v>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
         <v>0.90016387866794467</v>
       </c>
       <c r="S26" s="21">
-        <f t="shared" ref="S26" si="14">S3/R3-1</f>
+        <f t="shared" ref="S26" si="18">S3/R3-1</f>
         <v>1.1089625926721474</v>
       </c>
       <c r="T26" s="32"/>
@@ -2952,15 +2952,15 @@
         <v>1.2240730385914795</v>
       </c>
       <c r="K27" s="19">
-        <f t="shared" ref="K27:M27" si="15">K3/J3-1</f>
+        <f t="shared" ref="K27:M27" si="19">K3/J3-1</f>
         <v>-0.11856546770189635</v>
       </c>
       <c r="L27" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.11740031878812585</v>
       </c>
       <c r="M27" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>7.6692729281293781E-2</v>
       </c>
       <c r="Q27" s="28" t="s">
@@ -3049,11 +3049,11 @@
         <v>581.35500000000002</v>
       </c>
       <c r="R32" s="17">
-        <f t="shared" ref="R32:R57" si="16">F32</f>
+        <f t="shared" ref="R32:R57" si="20">F32</f>
         <v>287.71800000000002</v>
       </c>
       <c r="S32" s="17">
-        <f t="shared" ref="S32:S57" si="17">K32</f>
+        <f t="shared" ref="S32:S57" si="21">K32</f>
         <v>464.85399999999998</v>
       </c>
       <c r="T32" s="32"/>
@@ -3089,11 +3089,11 @@
         <v>89.453999999999994</v>
       </c>
       <c r="R33" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>30.248999999999999</v>
       </c>
       <c r="S33" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>55.945999999999998</v>
       </c>
       <c r="T33" s="32"/>
@@ -3128,11 +3128,11 @@
         <v>40.991</v>
       </c>
       <c r="R34" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>44.521999999999998</v>
       </c>
       <c r="S34" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>48.210999999999999</v>
       </c>
     </row>
@@ -3166,11 +3166,11 @@
         <v>98.626999999999995</v>
       </c>
       <c r="R35" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>14.558</v>
       </c>
       <c r="S35" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>56.561999999999998</v>
       </c>
     </row>
@@ -3182,20 +3182,20 @@
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18">
-        <f t="shared" ref="F36:J36" si="18">SUM(F31:F35)</f>
+        <f t="shared" ref="F36:J36" si="22">SUM(F31:F35)</f>
         <v>2194.3049999999998</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>3056.9639999999999</v>
       </c>
       <c r="I36" s="18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>2985.0720000000001</v>
       </c>
       <c r="J36" s="18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>2753.33</v>
       </c>
       <c r="K36" s="18">
@@ -3211,11 +3211,11 @@
         <v>2193.078</v>
       </c>
       <c r="R36" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>2194.3049999999998</v>
       </c>
       <c r="S36" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>2398.4649999999997</v>
       </c>
     </row>
@@ -3249,11 +3249,11 @@
         <v>58.225999999999999</v>
       </c>
       <c r="R37" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>40.826999999999998</v>
       </c>
       <c r="S37" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>49.734000000000002</v>
       </c>
     </row>
@@ -3294,11 +3294,11 @@
         <v>1682.6660000000002</v>
       </c>
       <c r="R38" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>1125.5329999999999</v>
       </c>
       <c r="S38" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1138.6779999999999</v>
       </c>
     </row>
@@ -3333,11 +3333,11 @@
         <v>74.703000000000003</v>
       </c>
       <c r="R39" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>68.076999999999998</v>
       </c>
       <c r="S39" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>61.168999999999997</v>
       </c>
     </row>
@@ -3371,11 +3371,11 @@
         <v>8.7460000000000004</v>
       </c>
       <c r="R40" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>2.9550000000000001</v>
       </c>
       <c r="S40" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>7.4740000000000002</v>
       </c>
     </row>
@@ -3409,11 +3409,11 @@
         <v>174.63399999999999</v>
       </c>
       <c r="R41" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>7.6319999999999997</v>
       </c>
       <c r="S41" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>90.795000000000002</v>
       </c>
       <c r="T41" s="32"/>
@@ -3426,20 +3426,20 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18">
-        <f t="shared" ref="F42" si="19">F36+SUM(F37:F41)</f>
+        <f t="shared" ref="F42" si="23">F36+SUM(F37:F41)</f>
         <v>3439.3289999999997</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="18">
-        <f t="shared" ref="H42:J42" si="20">H36+SUM(H37:H41)</f>
+        <f t="shared" ref="H42:J42" si="24">H36+SUM(H37:H41)</f>
         <v>4358.8559999999998</v>
       </c>
       <c r="I42" s="18">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>4259.4210000000003</v>
       </c>
       <c r="J42" s="18">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>4069.0540000000001</v>
       </c>
       <c r="K42" s="18">
@@ -3455,11 +3455,11 @@
         <v>4192.0529999999999</v>
       </c>
       <c r="R42" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>3439.3289999999997</v>
       </c>
       <c r="S42" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>3746.3149999999996</v>
       </c>
     </row>
@@ -3507,11 +3507,11 @@
         <v>560.79399999999998</v>
       </c>
       <c r="R44" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>223.63300000000001</v>
       </c>
       <c r="S44" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>379.25400000000002</v>
       </c>
     </row>
@@ -3545,11 +3545,11 @@
         <v>670.78399999999999</v>
       </c>
       <c r="R45" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>317.94200000000001</v>
       </c>
       <c r="S45" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>520.77499999999998</v>
       </c>
     </row>
@@ -3583,11 +3583,11 @@
         <v>5.6449999999999996</v>
       </c>
       <c r="R46" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>12.837</v>
       </c>
       <c r="S46" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>12.911</v>
       </c>
     </row>
@@ -3623,11 +3623,11 @@
         <v>47.951000000000001</v>
       </c>
       <c r="R47" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S47" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -3645,35 +3645,35 @@
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18">
-        <f>SUM(H44:H47)</f>
+        <f t="shared" ref="H48:M48" si="25">SUM(H44:H47)</f>
         <v>647.03</v>
       </c>
       <c r="I48" s="18">
-        <f>SUM(I44:I47)</f>
+        <f t="shared" si="25"/>
         <v>939.90800000000002</v>
       </c>
       <c r="J48" s="18">
-        <f>SUM(J44:J47)</f>
+        <f t="shared" si="25"/>
         <v>929.42500000000007</v>
       </c>
       <c r="K48" s="18">
-        <f>SUM(K44:K47)</f>
+        <f t="shared" si="25"/>
         <v>912.93999999999994</v>
       </c>
       <c r="L48" s="18">
-        <f>SUM(L44:L47)</f>
+        <f t="shared" si="25"/>
         <v>920.62900000000002</v>
       </c>
       <c r="M48" s="18">
-        <f>SUM(M44:M47)</f>
+        <f t="shared" si="25"/>
         <v>1285.174</v>
       </c>
       <c r="R48" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>554.41200000000003</v>
       </c>
       <c r="S48" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>912.93999999999994</v>
       </c>
     </row>
@@ -3708,11 +3708,11 @@
         <v>1250.434</v>
       </c>
       <c r="R49" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S49" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1249.106</v>
       </c>
       <c r="T49" s="32"/>
@@ -3747,11 +3747,11 @@
         <v>76.08</v>
       </c>
       <c r="R50" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>68.775000000000006</v>
       </c>
       <c r="S50" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>54.457000000000001</v>
       </c>
     </row>
@@ -3785,11 +3785,11 @@
         <v>19.876999999999999</v>
       </c>
       <c r="R51" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>65.444000000000003</v>
       </c>
       <c r="S51" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>14.23</v>
       </c>
     </row>
@@ -3823,11 +3823,11 @@
         <v>67.924999999999997</v>
       </c>
       <c r="R52" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>72.066000000000003</v>
       </c>
       <c r="S52" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>78.947000000000003</v>
       </c>
     </row>
@@ -3861,11 +3861,11 @@
         <v>57.447000000000003</v>
       </c>
       <c r="R53" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>47.286999999999999</v>
       </c>
       <c r="S53" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>51.034999999999997</v>
       </c>
     </row>
@@ -3877,20 +3877,20 @@
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18">
-        <f t="shared" ref="F54" si="21">F48+SUM(F49:F53)</f>
+        <f t="shared" ref="F54" si="26">F48+SUM(F49:F53)</f>
         <v>807.98400000000004</v>
       </c>
       <c r="G54" s="18"/>
       <c r="H54" s="18">
-        <f t="shared" ref="H54:J54" si="22">H48+SUM(H49:H53)</f>
+        <f t="shared" ref="H54:J54" si="27">H48+SUM(H49:H53)</f>
         <v>2153.5039999999999</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>2432.8900000000003</v>
       </c>
       <c r="J54" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>2390.5259999999998</v>
       </c>
       <c r="K54" s="18">
@@ -3906,11 +3906,11 @@
         <v>2756.9369999999999</v>
       </c>
       <c r="R54" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>807.98400000000004</v>
       </c>
       <c r="S54" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>2360.7150000000001</v>
       </c>
     </row>
@@ -3927,11 +3927,11 @@
       <c r="K55" s="18"/>
       <c r="M55" s="18"/>
       <c r="R55" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S55" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
         <v>2631.3449999999998</v>
       </c>
       <c r="S56" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1385.6</v>
       </c>
     </row>
@@ -3981,20 +3981,20 @@
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18">
-        <f t="shared" ref="F57" si="23">F56+F54</f>
+        <f t="shared" ref="F57" si="28">F56+F54</f>
         <v>3439.3289999999997</v>
       </c>
       <c r="G57" s="18"/>
       <c r="H57" s="18">
-        <f t="shared" ref="H57:J57" si="24">H56+H54</f>
+        <f t="shared" ref="H57:J57" si="29">H56+H54</f>
         <v>4358.8559999999998</v>
       </c>
       <c r="I57" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>4259.0570000000007</v>
       </c>
       <c r="J57" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>4069.0540000000001</v>
       </c>
       <c r="K57" s="18">
@@ -4010,11 +4010,11 @@
         <v>4192.0529999999999</v>
       </c>
       <c r="R57" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>3439.3289999999997</v>
       </c>
       <c r="S57" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>3746.3150000000001</v>
       </c>
     </row>
@@ -4023,36 +4023,36 @@
         <v>106</v>
       </c>
       <c r="H59" s="18">
-        <f t="shared" ref="H59:M59" si="25">H31-H44</f>
-        <v>2351.904</v>
+        <f t="shared" ref="H59:M59" si="30">H42-H54</f>
+        <v>2205.3519999999999</v>
       </c>
       <c r="I59" s="18">
-        <f t="shared" si="25"/>
-        <v>1978.3279999999997</v>
+        <f t="shared" si="30"/>
+        <v>1826.5309999999999</v>
       </c>
       <c r="J59" s="18">
-        <f t="shared" si="25"/>
-        <v>1765.1549999999997</v>
+        <f t="shared" si="30"/>
+        <v>1678.5280000000002</v>
       </c>
       <c r="K59" s="18">
-        <f t="shared" si="25"/>
-        <v>1393.6379999999999</v>
+        <f t="shared" si="30"/>
+        <v>1385.5999999999995</v>
       </c>
       <c r="L59" s="18">
-        <f t="shared" si="25"/>
-        <v>1099.691</v>
+        <f t="shared" si="30"/>
+        <v>1763.8839999999996</v>
       </c>
       <c r="M59" s="18">
-        <f>M31-M44</f>
-        <v>821.85700000000008</v>
+        <f>M42-M54</f>
+        <v>1435.116</v>
       </c>
       <c r="R59" s="18">
-        <f>R31-R44</f>
-        <v>1593.625</v>
+        <f>R42-R54</f>
+        <v>2631.3449999999998</v>
       </c>
       <c r="S59" s="18">
-        <f>S31-S44</f>
-        <v>1393.6379999999999</v>
+        <f>S42-S54</f>
+        <v>1385.5999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.15">
@@ -4060,28 +4060,28 @@
         <v>107</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" ref="H60:L60" si="26">H59/H19</f>
-        <v>5.8585666351971746</v>
+        <f t="shared" ref="H60:L60" si="31">H59/H19</f>
+        <v>5.4935072375680969</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" si="26"/>
-        <v>4.8987430790107069</v>
+        <f t="shared" si="31"/>
+        <v>4.5228627886015396</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="26"/>
-        <v>4.3192645998811026</v>
+        <f t="shared" si="31"/>
+        <v>4.1072917507579954</v>
       </c>
       <c r="K60" s="1">
-        <f t="shared" si="26"/>
-        <v>3.3903022872239497</v>
+        <f t="shared" si="31"/>
+        <v>3.370748249672801</v>
       </c>
       <c r="L60" s="1">
-        <f t="shared" si="26"/>
-        <v>2.4516803337426607</v>
+        <f t="shared" si="31"/>
+        <v>3.9324498552805633</v>
       </c>
       <c r="M60" s="1">
         <f>M59/M19</f>
-        <v>1.8310353832626747</v>
+        <v>3.1973301621649464</v>
       </c>
       <c r="R60" s="1" t="e">
         <f>R59/R19</f>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="S60" s="1">
         <f>S59/S19</f>
-        <v>3.4101771676986443</v>
+        <v>3.3905084990243086</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.15">
@@ -4097,23 +4097,23 @@
         <v>6</v>
       </c>
       <c r="H62" s="18">
-        <f t="shared" ref="H62:M62" si="27">H31</f>
+        <f t="shared" ref="H62:L62" si="32">H31</f>
         <v>2646.5</v>
       </c>
       <c r="I62" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>2394.8649999999998</v>
       </c>
       <c r="J62" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>2152.8919999999998</v>
       </c>
       <c r="K62" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>1772.8920000000001</v>
       </c>
       <c r="L62" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>1514.3710000000001</v>
       </c>
       <c r="M62" s="18">
@@ -4134,23 +4134,23 @@
         <v>7</v>
       </c>
       <c r="H63" s="18">
-        <f t="shared" ref="H63:M63" si="28">H49</f>
+        <f t="shared" ref="H63:L63" si="33">H49</f>
         <v>1247.1179999999999</v>
       </c>
       <c r="I63" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>1247.7850000000001</v>
       </c>
       <c r="J63" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>1248.452</v>
       </c>
       <c r="K63" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>1249.106</v>
       </c>
       <c r="L63" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>1249.7660000000001</v>
       </c>
       <c r="M63" s="18">
@@ -4171,23 +4171,23 @@
         <v>8</v>
       </c>
       <c r="H64" s="18">
-        <f t="shared" ref="H64:L64" si="29">H62-H63</f>
+        <f t="shared" ref="H64:L64" si="34">H62-H63</f>
         <v>1399.3820000000001</v>
       </c>
       <c r="I64" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>1147.0799999999997</v>
       </c>
       <c r="J64" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>904.43999999999983</v>
       </c>
       <c r="K64" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>523.78600000000006</v>
       </c>
       <c r="L64" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>264.60500000000002</v>
       </c>
       <c r="M64" s="18">
@@ -4240,27 +4240,27 @@
         <v>5</v>
       </c>
       <c r="F67" s="18">
-        <f t="shared" ref="F67:L67" si="30">F66*F19</f>
+        <f t="shared" ref="F67:L67" si="35">F66*F19</f>
         <v>0</v>
       </c>
       <c r="H67" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>20943.489990000002</v>
       </c>
       <c r="I67" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>19449.127039999999</v>
       </c>
       <c r="J67" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>11226.172124609999</v>
       </c>
       <c r="K67" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>8003.4550199999994</v>
       </c>
       <c r="L67" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>5234.5298827799998</v>
       </c>
       <c r="M67" s="18">
@@ -4281,27 +4281,27 @@
         <v>9</v>
       </c>
       <c r="F68" s="18">
-        <f t="shared" ref="F68:L68" si="31">F67-F64</f>
+        <f t="shared" ref="F68:L68" si="36">F67-F64</f>
         <v>0</v>
       </c>
       <c r="H68" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>19544.10799</v>
       </c>
       <c r="I68" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>18302.047040000001</v>
       </c>
       <c r="J68" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>10321.732124609998</v>
       </c>
       <c r="K68" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>7479.6690199999994</v>
       </c>
       <c r="L68" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>4969.9248827800002</v>
       </c>
       <c r="M68" s="18">
@@ -4321,57 +4321,57 @@
       <c r="B70" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F70" s="61"/>
-      <c r="H70" s="61">
-        <f t="shared" ref="F70:M70" si="32">H66/H60</f>
-        <v>8.9049085294297718</v>
-      </c>
-      <c r="I70" s="61">
-        <f t="shared" si="32"/>
-        <v>9.8310932464181864</v>
-      </c>
-      <c r="J70" s="61">
-        <f t="shared" si="32"/>
-        <v>6.3598789480867115</v>
-      </c>
-      <c r="K70" s="61">
-        <f t="shared" si="32"/>
-        <v>5.7428507402926723</v>
-      </c>
-      <c r="L70" s="61">
-        <f t="shared" si="32"/>
-        <v>4.7600006572573568</v>
-      </c>
-      <c r="M70" s="61">
+      <c r="F70" s="50"/>
+      <c r="H70" s="50">
+        <f t="shared" ref="H70:L70" si="37">H66/H60</f>
+        <v>9.4966653804018595</v>
+      </c>
+      <c r="I70" s="50">
+        <f t="shared" si="37"/>
+        <v>10.648123158052066</v>
+      </c>
+      <c r="J70" s="50">
+        <f t="shared" si="37"/>
+        <v>6.6881053664937351</v>
+      </c>
+      <c r="K70" s="50">
+        <f t="shared" si="37"/>
+        <v>5.7761655744803706</v>
+      </c>
+      <c r="L70" s="50">
+        <f t="shared" si="37"/>
+        <v>2.967615717802305</v>
+      </c>
+      <c r="M70" s="50">
         <f>M66/M60</f>
-        <v>8.268545839361348</v>
-      </c>
-      <c r="S70" s="61">
+        <v>4.7352006931147033</v>
+      </c>
+      <c r="S70" s="50">
         <f>S66/S60</f>
-        <v>4.4396520343302921</v>
+        <v>4.4654068864174388</v>
       </c>
     </row>
     <row r="71" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B71" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J71" s="61">
+      <c r="J71" s="50">
         <f>J67/SUM(G3:J3)</f>
         <v>8.6620027581335215</v>
       </c>
-      <c r="K71" s="61">
+      <c r="K71" s="50">
         <f>K67/SUM(H3:K3)</f>
         <v>5.7128606792228718</v>
       </c>
-      <c r="L71" s="61">
+      <c r="L71" s="50">
         <f>L67/SUM(I3:L3)</f>
         <v>3.3350853710591801</v>
       </c>
-      <c r="M71" s="61">
+      <c r="M71" s="50">
         <f>M67/SUM(J3:M3)</f>
         <v>3.6561758853858142</v>
       </c>
-      <c r="S71" s="61">
+      <c r="S71" s="50">
         <f>S67/S3</f>
         <v>4.7740342831504021</v>
       </c>
@@ -4380,25 +4380,25 @@
       <c r="B72" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H72" s="61"/>
-      <c r="I72" s="61"/>
-      <c r="J72" s="61">
-        <f t="shared" ref="H72:L72" si="33">J68/SUM(G3:J3)</f>
+      <c r="H72" s="50"/>
+      <c r="I72" s="50"/>
+      <c r="J72" s="50">
+        <f t="shared" ref="J72:L72" si="38">J68/SUM(G3:J3)</f>
         <v>7.964145849509074</v>
       </c>
-      <c r="K72" s="61">
-        <f t="shared" si="33"/>
+      <c r="K72" s="50">
+        <f t="shared" si="38"/>
         <v>5.3389825932900008</v>
       </c>
-      <c r="L72" s="61">
-        <f t="shared" si="33"/>
+      <c r="L72" s="50">
+        <f t="shared" si="38"/>
         <v>3.1664971149271057</v>
       </c>
-      <c r="M72" s="61">
+      <c r="M72" s="50">
         <f>M68/SUM(J3:M3)</f>
         <v>3.5850399606058789</v>
       </c>
-      <c r="S72" s="61">
+      <c r="S72" s="50">
         <f>S68/S3</f>
         <v>4.3698862150190001</v>
       </c>
@@ -4407,23 +4407,23 @@
       <c r="B73" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J73" s="61">
-        <f t="shared" ref="J73:L73" si="34">J66/SUM(G18:J18)</f>
+      <c r="J73" s="50">
+        <f t="shared" ref="J73:L73" si="39">J66/SUM(G18:J18)</f>
         <v>-7.2657282352914372</v>
       </c>
-      <c r="K73" s="61">
-        <f t="shared" si="34"/>
+      <c r="K73" s="50">
+        <f t="shared" si="39"/>
         <v>-4.8380279709585396</v>
       </c>
-      <c r="L73" s="61">
-        <f t="shared" si="34"/>
+      <c r="L73" s="50">
+        <f t="shared" si="39"/>
         <v>-3.1142253716484478</v>
       </c>
-      <c r="M73" s="61">
+      <c r="M73" s="50">
         <f>M66/SUM(J18:M18)</f>
         <v>-4.4911153824345522</v>
       </c>
-      <c r="S73" s="61">
+      <c r="S73" s="50">
         <f>S66/S18</f>
         <v>-4.0620326234132866</v>
       </c>

</xml_diff>